<commit_message>
Slight correction to weights
</commit_message>
<xml_diff>
--- a/corpus/weights.xlsx
+++ b/corpus/weights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rabraham5/Documents/Github/keygen-ronalabraham/corpus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902BC0D1-A7D0-CA46-9128-5D30037FEC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFCA1B1-C1EA-664C-80D3-9B5859DA454B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="8300" windowWidth="28800" windowHeight="20500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="29300" windowWidth="33600" windowHeight="20500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Penalty" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Old--Same Finger + Long Jump'!$A$2:$I$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2840,8 +2839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4715C5BF-7BAB-314B-95FF-5EF7930FFEFC}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2976,11 +2975,11 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <f t="shared" ref="P2:P16" si="0">V2+W2</f>
+        <f>V2+W2</f>
         <v>3</v>
       </c>
       <c r="Q2">
-        <f t="shared" ref="Q2:Q16" si="1">T2+U2</f>
+        <f>T2+U2</f>
         <v>10</v>
       </c>
       <c r="R2">
@@ -3040,11 +3039,11 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <f t="shared" si="0"/>
+        <f>V3+W3</f>
         <v>2</v>
       </c>
       <c r="Q3">
-        <f t="shared" si="1"/>
+        <f>T3+U3</f>
         <v>10</v>
       </c>
       <c r="R3">
@@ -3074,11 +3073,11 @@
         <v>1</v>
       </c>
       <c r="P4">
-        <f t="shared" si="0"/>
+        <f>V4+W4</f>
         <v>7</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="1"/>
+        <f>T4+U4</f>
         <v>10</v>
       </c>
       <c r="R4">
@@ -3108,11 +3107,11 @@
         <v>3</v>
       </c>
       <c r="P5">
-        <f t="shared" si="0"/>
+        <f>V5+W5</f>
         <v>8</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="1"/>
+        <f>T5+U5</f>
         <v>10</v>
       </c>
       <c r="R5">
@@ -3136,24 +3135,24 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="N6" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P6">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>V6+W6</f>
+        <v>5</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="1"/>
+        <f>T6+U6</f>
         <v>5</v>
       </c>
       <c r="R6">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="S6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T6">
         <v>5</v>
@@ -3162,32 +3161,35 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W6">
         <v>0</v>
+      </c>
+      <c r="X6" s="15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="N7" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <f>V7+W7</f>
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <f>T7+U7</f>
         <v>5</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
       <c r="R7">
-        <v>1</v>
+        <v>1.4</v>
       </c>
       <c r="S7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T7">
         <v>5</v>
@@ -3196,13 +3198,10 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W7">
         <v>0</v>
-      </c>
-      <c r="X7" s="15" t="s">
-        <v>24</v>
       </c>
       <c r="Y7" t="s">
         <v>156</v>
@@ -3216,11 +3215,11 @@
         <v>6</v>
       </c>
       <c r="P8">
-        <f t="shared" si="0"/>
+        <f>V8+W8</f>
         <v>14</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="1"/>
+        <f>T8+U8</f>
         <v>20</v>
       </c>
       <c r="R8">
@@ -3250,11 +3249,11 @@
         <v>7</v>
       </c>
       <c r="P9">
-        <f t="shared" si="0"/>
+        <f>V9+W9</f>
         <v>11</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="1"/>
+        <f>T9+U9</f>
         <v>10</v>
       </c>
       <c r="R9">
@@ -3284,11 +3283,11 @@
         <v>8</v>
       </c>
       <c r="P10">
-        <f t="shared" si="0"/>
+        <f>V10+W10</f>
         <v>15</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
+        <f>T10+U10</f>
         <v>15</v>
       </c>
       <c r="R10">
@@ -3324,11 +3323,11 @@
         <v>10</v>
       </c>
       <c r="P11">
-        <f t="shared" si="0"/>
+        <f>V11+W11</f>
         <v>13</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="1"/>
+        <f>T11+U11</f>
         <v>10</v>
       </c>
       <c r="R11">
@@ -3358,11 +3357,11 @@
         <v>10</v>
       </c>
       <c r="P12">
-        <f t="shared" si="0"/>
+        <f>V12+W12</f>
         <v>17</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="1"/>
+        <f>T12+U12</f>
         <v>10</v>
       </c>
       <c r="R12">
@@ -3392,11 +3391,11 @@
         <v>15</v>
       </c>
       <c r="P13">
-        <f t="shared" si="0"/>
+        <f>V13+W13</f>
         <v>18</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="1"/>
+        <f>T13+U13</f>
         <v>15</v>
       </c>
       <c r="R13">
@@ -3426,11 +3425,11 @@
         <v>15</v>
       </c>
       <c r="P14">
-        <f t="shared" si="0"/>
+        <f>V14+W14</f>
         <v>20</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="1"/>
+        <f>T14+U14</f>
         <v>15</v>
       </c>
       <c r="R14">
@@ -3460,11 +3459,11 @@
         <v>20</v>
       </c>
       <c r="P15">
-        <f t="shared" si="0"/>
+        <f>V15+W15</f>
         <v>25</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="1"/>
+        <f>T15+U15</f>
         <v>25</v>
       </c>
       <c r="R15">
@@ -3494,11 +3493,11 @@
         <v>25</v>
       </c>
       <c r="P16">
-        <f t="shared" si="0"/>
+        <f>V16+W16</f>
         <v>28</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="1"/>
+        <f>T16+U16</f>
         <v>20</v>
       </c>
       <c r="R16">
@@ -3523,7 +3522,7 @@
     <row r="17" spans="15:17" x14ac:dyDescent="0.2">
       <c r="O17">
         <f>SUM(O2:O16)</f>
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P17">
         <f>SUM(P2:P16)</f>
@@ -3535,11 +3534,11 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N2:W16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N2:X16">
     <sortCondition ref="O2:O16"/>
   </sortState>
   <conditionalFormatting sqref="P2:Q16">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3549,7 +3548,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O16">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3564,10 +3563,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7AFBDD1-7053-044C-A762-00CA2082A921}">
-  <dimension ref="A1:S60"/>
+  <dimension ref="A1:R60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3579,12 +3578,11 @@
     <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="27.1640625" customWidth="1"/>
-    <col min="10" max="21" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="27.1640625" customWidth="1"/>
+    <col min="9" max="20" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>145</v>
       </c>
@@ -3607,9 +3605,8 @@
         <v>172</v>
       </c>
       <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -3631,9 +3628,9 @@
       <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="S2" s="5"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3656,7 +3653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>103</v>
       </c>
@@ -3679,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>119</v>
       </c>
@@ -3702,7 +3699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>108</v>
       </c>
@@ -3725,7 +3722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>126</v>
       </c>
@@ -3748,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>116</v>
       </c>
@@ -3771,7 +3768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -3794,7 +3791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>144</v>
       </c>
@@ -3817,7 +3814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>112</v>
       </c>
@@ -3840,7 +3837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>123</v>
       </c>
@@ -3863,7 +3860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>102</v>
       </c>
@@ -3886,7 +3883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>118</v>
       </c>
@@ -3909,7 +3906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
         <v>107</v>
       </c>
@@ -3932,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>125</v>
       </c>
@@ -4669,23 +4666,23 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>89</v>
+      <c r="A48" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D48" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E48" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F48" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G48" s="4">
         <v>4</v>
@@ -4693,7 +4690,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
         <v>97</v>
@@ -4715,8 +4712,8 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
-        <v>120</v>
+      <c r="A50" t="s">
+        <v>113</v>
       </c>
       <c r="B50" t="s">
         <v>97</v>
@@ -4734,24 +4731,24 @@
         <v>3</v>
       </c>
       <c r="G50" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="B51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C51" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D51" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E51" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F51" s="4">
         <v>3</v>
@@ -4762,25 +4759,25 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D52" s="4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E52" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F52" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G52" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -4968,11 +4965,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G60" xr:uid="{B7AFBDD1-7053-044C-A762-00CA2082A921}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G60">
-      <sortCondition ref="G1:G60"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:G60" xr:uid="{B7AFBDD1-7053-044C-A762-00CA2082A921}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>